<commit_message>
Excel sheet of discount updated
</commit_message>
<xml_diff>
--- a/DAY_8/Book3excel sheet.xlsx
+++ b/DAY_8/Book3excel sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE761AB8-752F-45FB-AE2F-A686FB2248AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BF811-C539-4AAF-8A01-EE152F133B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FFDC954A-FC81-4557-AE4E-5F606A56C6F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Hosteller Female working  &lt; 45</t>
   </si>
@@ -81,29 +81,38 @@
     <t>Senior citizen discount applied</t>
   </si>
   <si>
-    <t xml:space="preserve">Nykaa discount
+    <t>senior citizen discount applied</t>
+  </si>
+  <si>
+    <t>senior citizen discount</t>
+  </si>
+  <si>
+    <t>nykaa discount</t>
+  </si>
+  <si>
+    <t>nykaa discount,500 coupon for book</t>
+  </si>
+  <si>
+    <t>100  voucher in fastrack</t>
+  </si>
+  <si>
+    <t>100 voucher in fastrack,500 coupon for book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 voucher fastrack coupon  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Output
 </t>
   </si>
   <si>
-    <t>senior citizen discount applied</t>
-  </si>
-  <si>
-    <t>senior citizen discount</t>
-  </si>
-  <si>
-    <t>nykaa discount</t>
-  </si>
-  <si>
-    <t>nykaa discount,500 coupon for book</t>
-  </si>
-  <si>
-    <t>100  voucher in fastrack</t>
-  </si>
-  <si>
-    <t>100 voucher in fastrack,500 coupon for book</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 voucher fastrack coupon  </t>
+    <t>Nykaa discount applied</t>
+  </si>
+  <si>
+    <t>Actual output</t>
+  </si>
+  <si>
+    <t>Usecase</t>
   </si>
 </sst>
 </file>
@@ -461,137 +470,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DB3841-B91A-420B-B72E-7AFDF5DAFCA9}">
-  <dimension ref="I1:J15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="4" width="0.140625" customWidth="1"/>
+    <col min="5" max="5" width="0.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
+    <col min="9" max="9" width="31" customWidth="1"/>
+    <col min="10" max="11" width="63.7109375" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="9:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="9:11" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1" s="2" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="9:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="9:10" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="9:10" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>